<commit_message>
Perubahan Import Umat (lingkungan&kbg)
</commit_message>
<xml_diff>
--- a/core-sistem/public/template/kbg.xlsx
+++ b/core-sistem/public/template/kbg.xlsx
@@ -1,32 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\laravel\edo\sistem-informasi-gereja\core-sistem\public\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51356997-F5EF-4E67-9400-8E5176416A8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{123A412E-3527-4285-B6E3-AAB6C371BABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="1680" windowWidth="21600" windowHeight="13935" xr2:uid="{44FFA9F2-9BDD-4E6D-BC1B-1E5FC3E321B6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -41,33 +33,26 @@
     <t>hubungan</t>
   </si>
   <si>
+    <t>jenis_kelamin</t>
+  </si>
+  <si>
+    <t>lingkungan</t>
+  </si>
+  <si>
+    <t>kbg</t>
+  </si>
+  <si>
     <t>alamat</t>
   </si>
   <si>
     <t>telepon</t>
-  </si>
-  <si>
-    <t>jenis_kelamin</t>
-  </si>
-  <si>
-    <t>nama_lingkungan</t>
-  </si>
-  <si>
-    <t>nama_kbg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,18 +61,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -99,17 +78,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="40% - Accent3" xfId="1" builtinId="39"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -142,7 +117,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -154,7 +129,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -201,23 +176,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -253,23 +211,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -421,146 +362,46 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7940AB6-09D2-4F04-8472-C52994D629FF}">
-  <dimension ref="A1:M11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1"/>
+      <selection activeCell="A2" sqref="A2:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" customWidth="1"/>
-    <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" customWidth="1"/>
-    <col min="9" max="9" width="26.28515625" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" customWidth="1"/>
+    <col min="5" max="5" width="26.28515625" customWidth="1"/>
+    <col min="6" max="6" width="34.7109375" customWidth="1"/>
+    <col min="7" max="7" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>